<commit_message>
动态规划 - coins in a line
</commit_message>
<xml_diff>
--- a/src/test/java/cn/juntaozhang/lintcode/CoinsInALine.xlsx
+++ b/src/test/java/cn/juntaozhang/lintcode/CoinsInALine.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juntao/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juntaozhang/src/juntaozhang/LintCode/src/test/java/cn/juntaozhang/lintcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16140" tabRatio="500"/>
+    <workbookView xWindow="29980" yWindow="3340" windowWidth="28800" windowHeight="16140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>values</t>
   </si>
@@ -37,12 +37,31 @@
   <si>
     <t>dp</t>
   </si>
+  <si>
+    <t>6=max(9-3,9-7)</t>
+  </si>
+  <si>
+    <t>6=max(1+min(7,5),1+1+min(5,0))</t>
+  </si>
+  <si>
+    <t>dp[i] = Math.max(sum[i] - dp[i + 1], sum[i] - dp[i + 2]);
+dp[i] = Math.max(
+        values[i] + Math.min(dp[i + 2], dp[i + 3]), 
+        values[i] + values[i + 1] + Math.min(dp[i + 3], dp[i + 4])
+     );
+dp[i]=&gt;从i到end的最大值
+sum[i] - dp[i + 1]  =&gt; values[i] + min(dp[i + 2], dp[i + 3])
+sum[i] - dp[i + 2]  =&gt; values[i] + values[i + 1] + min(dp[i + 3], dp[i + 4])</t>
+  </si>
+  <si>
+    <t>II</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -55,6 +74,14 @@
       <sz val="12"/>
       <color theme="4" tint="0.39997558519241921"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -78,9 +105,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -358,77 +395,262 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D2:H5"/>
+  <dimension ref="C4:R20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="7" max="7" width="11.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="E2" s="1">
+    <row r="4" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C4" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C5" s="4"/>
+    </row>
+    <row r="6" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C6" s="4"/>
+    </row>
+    <row r="7" spans="3:18" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C7" s="4"/>
+      <c r="K7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+    </row>
+    <row r="8" spans="3:18" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C8" s="4"/>
+      <c r="E8" s="1">
         <v>0</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F8" s="1">
         <v>1</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G8" s="1">
         <v>2</v>
       </c>
-      <c r="H2" s="1">
+      <c r="H8" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D3" t="s">
+      <c r="I8" s="1">
+        <v>4</v>
+      </c>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+    </row>
+    <row r="9" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C9" s="4"/>
+      <c r="D9" t="s">
         <v>0</v>
       </c>
-      <c r="E3">
+      <c r="E9" s="5">
         <v>1</v>
       </c>
-      <c r="F3">
+      <c r="F9" s="5">
+        <v>1</v>
+      </c>
+      <c r="G9" s="5">
         <v>2</v>
       </c>
-      <c r="G3">
+      <c r="H9" s="5">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D4" t="s">
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+    </row>
+    <row r="10" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C10" s="4"/>
+      <c r="D10" t="s">
         <v>1</v>
       </c>
-      <c r="E4">
+      <c r="E10">
+        <v>9</v>
+      </c>
+      <c r="F10">
+        <v>8</v>
+      </c>
+      <c r="G10">
+        <v>7</v>
+      </c>
+      <c r="H10">
+        <v>5</v>
+      </c>
+      <c r="I10">
         <v>0</v>
       </c>
-      <c r="F4">
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
+    </row>
+    <row r="11" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C11" s="4"/>
+      <c r="D11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <v>6</v>
+      </c>
+      <c r="F11">
+        <v>3</v>
+      </c>
+      <c r="G11">
+        <v>7</v>
+      </c>
+      <c r="H11">
         <v>5</v>
       </c>
-      <c r="G4">
-        <v>7</v>
-      </c>
-      <c r="H4">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5">
+      <c r="I11">
         <v>0</v>
       </c>
-      <c r="F5">
-        <v>5</v>
-      </c>
-      <c r="G5">
-        <v>7</v>
-      </c>
-      <c r="H5">
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
+    </row>
+    <row r="12" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C12" s="4"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
+    </row>
+    <row r="13" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C13" s="4"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3"/>
+    </row>
+    <row r="14" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C14" s="4"/>
+      <c r="E14" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="3"/>
+    </row>
+    <row r="15" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C15" s="4"/>
+      <c r="E15" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="3"/>
+      <c r="R15" s="3"/>
+    </row>
+    <row r="16" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+      <c r="P16" s="3"/>
+      <c r="Q16" s="3"/>
+      <c r="R16" s="3"/>
+    </row>
+    <row r="17" spans="11:18" x14ac:dyDescent="0.2">
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="3"/>
+      <c r="R17" s="3"/>
+    </row>
+    <row r="18" spans="11:18" x14ac:dyDescent="0.2">
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+      <c r="P18" s="3"/>
+      <c r="Q18" s="3"/>
+      <c r="R18" s="3"/>
+    </row>
+    <row r="19" spans="11:18" x14ac:dyDescent="0.2">
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+      <c r="P19" s="3"/>
+      <c r="Q19" s="3"/>
+      <c r="R19" s="3"/>
+    </row>
+    <row r="20" spans="11:18" x14ac:dyDescent="0.2">
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+      <c r="P20" s="3"/>
+      <c r="Q20" s="3"/>
+      <c r="R20" s="3"/>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="C4:C15"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="K7:R20"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>